<commit_message>
_01_TEST 3 FARKLI TEST SENARYOSU bitmiştir by Ahmet
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="8">
   <si>
     <t>Fee Functionality</t>
   </si>
@@ -30,6 +30,12 @@
   </si>
   <si>
     <t>Admin User should be able to Add Subject Categories</t>
+  </si>
+  <si>
+    <t>Human Resources  Position Catagories Add Functionality</t>
+  </si>
+  <si>
+    <t>Human Resources  PositionCatagories Delete Functionality</t>
   </si>
 </sst>
 </file>
@@ -74,7 +80,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -179,6 +185,160 @@
         <v>2</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>